<commit_message>
Pick Up And Haul 업데이트
</commit_message>
<xml_diff>
--- a/Data/Pick Up And Haul - 1279012058/1279012058.xlsx
+++ b/Data/Pick Up And Haul - 1279012058/1279012058.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Pick Up And Haul - 1279012058\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Pick Up And Haul - 1279012058\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5AAB40-51ED-4BDE-8DE3-EA01238E0914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB21FA6D-E4CD-4853-A251-B08B6981186A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Merge" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_231218" sheetId="3" r:id="rId1"/>
+    <sheet name="231215" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,6 +39,1418 @@
     <author>강석진</author>
   </authors>
   <commentList>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{555DF975-7F52-4521-BFD9-D4BE86516562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>반드시</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>맨</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>앞에</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>한</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>칸</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>띄우기</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{5442A698-17A0-4C4C-846A-0C42C63037D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>소지품에</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>넣는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>것</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>뿐</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>아니라</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>저장구역에</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>도달하는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>것</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>까지</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">포함됨
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>바닐라</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기본</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">)TargetA </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>중</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{464DA4CC-7812-4EA1-8D9A-D0E843571665}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>훈련이</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>가능한</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>똑똑함</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>지능</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>수준과</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>짐꾼</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사용</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>가능</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>속성이</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모두</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>필요함</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E78B4E0E-8769-4E8E-8E4A-572F71AE595E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>옛날에는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>메카노이드를</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>조종하는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>컨텐츠의</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대명사가</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> What The Hack </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이라는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모드였음
+지금은</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>바이오테크도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>있고</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>해서</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>언급할거면</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>차라리</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이쪽이</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>나음</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{49C14B76-9D56-4A22-82B7-AB161E9B4257}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>최신</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>바닐라에선</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>같은</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>종류의</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>물건끼리는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모아서</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>옮기도록</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">바뀜
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PUAH</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>의</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모아서</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반하기</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>소지품</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>공간</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사용해서</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반하기에서
+모아서</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>운반하기가</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>바닐라</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기능으로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>빠졌다고</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>보면</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>됨</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>강석진</author>
+  </authors>
+  <commentList>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{22F7AE1F-CEB5-4994-8BE8-022707FF435C}">
       <text>
         <r>
@@ -1340,7 +2752,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1588,6 +3000,10 @@
   </si>
   <si>
     <t>기본값: 켜짐\n\n이 옵션을 키면 운반 훈련이 완료된 짐꾼 동물이 운반할 때 소지품 공간을 활용할 수 있습니다.\n\n바닐라 림월드에서 이 기능을 활용할 수 있는 동물은 코끼리와 트럼보 및 이데올로기 DLC의 짐꾼 나무지기밖에 없기 때문에, VFME와 같이 짐꾼 동물을 확장하는 모드와 함께 사용하는 것이 좋습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetA 모아서 운반 중</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2036,11 +3452,288 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DECFBED-9A06-41BB-82AA-C71BFB361A66}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="57.9140625" customWidth="1"/>
+    <col min="6" max="6" width="29.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2096,9 +3789,8 @@
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="str">
-        <f>IFERROR(VLOOKUP(A2,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>소지품에 모아서 운반</v>
+      <c r="G2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2118,9 +3810,8 @@
       <c r="F3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="str">
-        <f>IFERROR(VLOOKUP(A3,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>운반</v>
+      <c r="G3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
@@ -2142,9 +3833,8 @@
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="str">
-        <f>IFERROR(VLOOKUP(A4,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>모아서 운반</v>
+      <c r="G4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -2166,9 +3856,8 @@
       <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="str">
-        <f>IFERROR(VLOOKUP(A5,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>TargetA(을)를 운반하기 위해 소지품에 넣는 중.</v>
+      <c r="G5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -2187,9 +3876,8 @@
       <c r="E6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G6" t="str">
-        <f>IFERROR(VLOOKUP(A6,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>소지품에서 꺼내는 중.</v>
+      <c r="G6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -2208,9 +3896,8 @@
       <c r="E7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G7" t="str">
-        <f>IFERROR(VLOOKUP(A7,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>시신을 소지품에 넣는 것을 허용</v>
+      <c r="G7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -2229,9 +3916,8 @@
       <c r="E8" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G8" t="str">
-        <f>IFERROR(VLOOKUP(A8,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>기본값 꺼짐. 손에 직접 들고 다니십시오.</v>
+      <c r="G8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -2250,9 +3936,8 @@
       <c r="E9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G9" t="str">
-        <f>IFERROR(VLOOKUP(A9,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>길들여진 동물들이 소지품 공간을 사용해서 운반 허용</v>
+      <c r="G9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -2271,9 +3956,8 @@
       <c r="E10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G10" t="str">
-        <f>IFERROR(VLOOKUP(A10,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>기본값 켜짐. VFME 캐러밴 팩과 같이 더 많은 동물에게 배낭을 제공하는 모드와 같이 사용하는게 제일 좋습니다.</v>
+      <c r="G10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -2292,9 +3976,8 @@
       <c r="E11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G11" t="str">
-        <f>IFERROR(VLOOKUP(A11,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>해킹된 메카노이드가 소지품 공간을 사용해서 운반하도록 허용</v>
+      <c r="G11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -2313,9 +3996,8 @@
       <c r="E12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G12" t="str">
-        <f>IFERROR(VLOOKUP(A12,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>기본값 켜짐. WTH 또는 이와 유사한 모드가 필요합니다.</v>
+      <c r="G12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -2334,9 +4016,8 @@
       <c r="E13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G13" t="str">
-        <f>IFERROR(VLOOKUP(A13,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>소지품 공간을 이용해서 운반 시 최소 여유 공간</v>
+      <c r="G13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -2355,9 +4036,8 @@
       <c r="E14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G14" t="str">
-        <f>IFERROR(VLOOKUP(A14,Merge!$C$2:$D$14,2,FALSE),"")</f>
-        <v>기본 값 20%. 설정 값보다 여유 공간이 적을 경우 림월드의 기본 운반 시스템을 사용하여 직접 들고 옵니다. 0%로 설정 시 감자 두개가 들어갈 공간이 있는지 확인하지 않고 무조건 소지품 창에 집어넣고 운반합니다. 100%로 설정 시 정착민이 자신의 옷을 다 벗어버리는 결과를 가져옵니다.</v>
+      <c r="G14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45"/>
@@ -2366,128 +4046,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5808668-0080-4FB3-9D8D-AEB99E1EFA26}">
-  <dimension ref="C2:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>